<commit_message>
feat: set up initial component architecture
</commit_message>
<xml_diff>
--- a/Model_Param_Tracking.xlsx
+++ b/Model_Param_Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlotte/Desktop/Dissertation_Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7C24910A-42E8-B640-988D-1976760746AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2A775BC8-F713-D344-B9FB-088552282622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3600" windowWidth="38400" windowHeight="21600" xr2:uid="{93C3F197-1E59-6347-8491-F25656B50BA9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{93C3F197-1E59-6347-8491-F25656B50BA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Param_Tracking" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="83">
   <si>
     <t>heads_gat</t>
   </si>
@@ -243,6 +243,48 @@
   </si>
   <si>
     <t>lambda_mean_align</t>
+  </si>
+  <si>
+    <t>20250912_151512</t>
+  </si>
+  <si>
+    <t>Less var, more random spiking</t>
+  </si>
+  <si>
+    <t>20250812_175431</t>
+  </si>
+  <si>
+    <t>Closer Corr (than even best), higher var</t>
+  </si>
+  <si>
+    <t>20250812_191550</t>
+  </si>
+  <si>
+    <t>Lambda mean does not work</t>
+  </si>
+  <si>
+    <t>20250813_</t>
+  </si>
+  <si>
+    <t>20250813_002441</t>
+  </si>
+  <si>
+    <t>20250813_011021</t>
+  </si>
+  <si>
+    <t>20250813_123507</t>
+  </si>
+  <si>
+    <t>Basically purely cyclical</t>
+  </si>
+  <si>
+    <t>20250813_124314</t>
+  </si>
+  <si>
+    <t>20250813_124436</t>
+  </si>
+  <si>
+    <t>High Var</t>
   </si>
 </sst>
 </file>
@@ -857,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BF201A-EBF7-3F4F-9E79-53BC4C3A4D14}">
   <dimension ref="B3:Z311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Y31" sqref="Y31"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="83" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2598,7 +2640,9 @@
       <c r="C27" s="18">
         <v>777885</v>
       </c>
-      <c r="D27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="E27" s="5" t="s">
         <v>46</v>
       </c>
@@ -2656,171 +2700,502 @@
       <c r="W27" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="X27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y27" s="10" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="28" spans="2:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="18"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="16"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
-      <c r="V28" s="9"/>
-      <c r="W28" s="8"/>
+      <c r="C28" s="18">
+        <v>777938</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="7">
+        <v>12</v>
+      </c>
+      <c r="G28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="H28" s="7">
+        <v>64</v>
+      </c>
+      <c r="I28" s="7">
+        <v>64</v>
+      </c>
+      <c r="J28" s="7">
+        <v>2</v>
+      </c>
+      <c r="K28" s="7">
+        <v>1</v>
+      </c>
+      <c r="L28" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="M28" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="N28" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="O28" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="P28" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>30</v>
+      </c>
+      <c r="R28" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="S28" s="7">
+        <v>8</v>
+      </c>
+      <c r="T28" s="16">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="U28" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="V28" s="9">
+        <v>1</v>
+      </c>
+      <c r="W28" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="X28" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y28" s="10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="29" spans="2:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="18"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="7"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="8"/>
+      <c r="C29" s="18">
+        <v>777952</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="7">
+        <v>12</v>
+      </c>
+      <c r="G29" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="H29" s="7">
+        <v>64</v>
+      </c>
+      <c r="I29" s="7">
+        <v>64</v>
+      </c>
+      <c r="J29" s="7">
+        <v>2</v>
+      </c>
+      <c r="K29" s="7">
+        <v>1</v>
+      </c>
+      <c r="L29" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="M29" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="N29" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="O29" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="P29" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>30</v>
+      </c>
+      <c r="R29" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="S29" s="7">
+        <v>8</v>
+      </c>
+      <c r="T29" s="16">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="U29" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="V29" s="9">
+        <v>1</v>
+      </c>
+      <c r="W29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="X29" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y29" s="10" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="30" spans="2:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="18"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="7"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="7"/>
-      <c r="V30" s="9"/>
-      <c r="W30" s="8"/>
+      <c r="C30" s="18">
+        <v>778024</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" s="7">
+        <v>12</v>
+      </c>
+      <c r="G30" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="H30" s="7">
+        <v>64</v>
+      </c>
+      <c r="I30" s="7">
+        <v>64</v>
+      </c>
+      <c r="J30" s="7">
+        <v>2</v>
+      </c>
+      <c r="K30" s="7">
+        <v>1</v>
+      </c>
+      <c r="L30" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="M30" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="N30" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="O30" s="13">
+        <v>0.03</v>
+      </c>
+      <c r="P30" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="7">
+        <v>30</v>
+      </c>
+      <c r="R30" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="S30" s="7">
+        <v>8</v>
+      </c>
+      <c r="T30" s="16">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="U30" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="V30" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="W30" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="X30" s="10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="31" spans="2:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="18"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="16"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="7"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="8"/>
+      <c r="C31" s="18">
+        <v>778028</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="7">
+        <v>12</v>
+      </c>
+      <c r="G31" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="H31" s="7">
+        <v>64</v>
+      </c>
+      <c r="I31" s="7">
+        <v>64</v>
+      </c>
+      <c r="J31" s="7">
+        <v>2</v>
+      </c>
+      <c r="K31" s="7">
+        <v>1</v>
+      </c>
+      <c r="L31" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="M31" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="N31" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="O31" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="P31" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="7">
+        <v>30</v>
+      </c>
+      <c r="R31" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="S31" s="7">
+        <v>8</v>
+      </c>
+      <c r="T31" s="16">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="U31" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="V31" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="W31" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="X31" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y31" s="10" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="32" spans="2:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="18"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="7"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="7"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="8"/>
-    </row>
-    <row r="33" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="18"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="7"/>
-      <c r="V33" s="9"/>
-      <c r="W33" s="8"/>
-    </row>
-    <row r="34" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C34" s="18"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="16"/>
-      <c r="S34" s="7"/>
-      <c r="T34" s="7"/>
-      <c r="U34" s="7"/>
-      <c r="V34" s="9"/>
-      <c r="W34" s="8"/>
-    </row>
-    <row r="35" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="18"/>
-      <c r="D35" s="5"/>
+      <c r="C32" s="18">
+        <v>778342</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="7">
+        <v>12</v>
+      </c>
+      <c r="G32" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="H32" s="7">
+        <v>64</v>
+      </c>
+      <c r="I32" s="7">
+        <v>64</v>
+      </c>
+      <c r="J32" s="7">
+        <v>2</v>
+      </c>
+      <c r="K32" s="7">
+        <v>1</v>
+      </c>
+      <c r="L32" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="M32" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="N32" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="O32" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="P32" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>30</v>
+      </c>
+      <c r="R32" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="S32" s="7">
+        <v>8</v>
+      </c>
+      <c r="T32" s="16">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="U32" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="V32" s="9">
+        <v>1</v>
+      </c>
+      <c r="W32" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="18">
+        <v>778349</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="7">
+        <v>12</v>
+      </c>
+      <c r="G33" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="H33" s="7">
+        <v>64</v>
+      </c>
+      <c r="I33" s="7">
+        <v>64</v>
+      </c>
+      <c r="J33" s="7">
+        <v>2</v>
+      </c>
+      <c r="K33" s="7">
+        <v>1</v>
+      </c>
+      <c r="L33" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="M33" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="N33" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="O33" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="P33" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="7">
+        <v>30</v>
+      </c>
+      <c r="R33" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="S33" s="7">
+        <v>8</v>
+      </c>
+      <c r="T33" s="16">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="U33" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="V33" s="9">
+        <v>1</v>
+      </c>
+      <c r="W33" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="X33" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y33" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="18">
+        <v>778350</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="7">
+        <v>12</v>
+      </c>
+      <c r="G34" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="H34" s="7">
+        <v>64</v>
+      </c>
+      <c r="I34" s="7">
+        <v>64</v>
+      </c>
+      <c r="J34" s="7">
+        <v>2</v>
+      </c>
+      <c r="K34" s="7">
+        <v>1</v>
+      </c>
+      <c r="L34" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="M34" s="7">
+        <v>1.5E-3</v>
+      </c>
+      <c r="N34" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="O34" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="P34" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="7">
+        <v>30</v>
+      </c>
+      <c r="R34" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="S34" s="7">
+        <v>8</v>
+      </c>
+      <c r="T34" s="16">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="U34" s="16">
+        <v>1E-4</v>
+      </c>
+      <c r="V34" s="9">
+        <v>1</v>
+      </c>
+      <c r="W34" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="18">
+        <v>778537</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="E35" s="5"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
@@ -2841,7 +3216,7 @@
       <c r="V35" s="9"/>
       <c r="W35" s="8"/>
     </row>
-    <row r="36" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="18"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -2864,7 +3239,7 @@
       <c r="V36" s="9"/>
       <c r="W36" s="7"/>
     </row>
-    <row r="37" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" s="18"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -2887,7 +3262,7 @@
       <c r="V37" s="9"/>
       <c r="W37" s="7"/>
     </row>
-    <row r="38" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C38" s="18"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
@@ -2910,7 +3285,7 @@
       <c r="V38" s="9"/>
       <c r="W38" s="7"/>
     </row>
-    <row r="39" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C39" s="18"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
@@ -2933,7 +3308,7 @@
       <c r="V39" s="9"/>
       <c r="W39" s="7"/>
     </row>
-    <row r="40" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="18"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -2956,7 +3331,7 @@
       <c r="V40" s="7"/>
       <c r="W40" s="7"/>
     </row>
-    <row r="41" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="18"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -2979,7 +3354,7 @@
       <c r="V41" s="7"/>
       <c r="W41" s="7"/>
     </row>
-    <row r="42" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="18"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -3002,7 +3377,7 @@
       <c r="V42" s="7"/>
       <c r="W42" s="7"/>
     </row>
-    <row r="43" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="18"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -3025,7 +3400,7 @@
       <c r="V43" s="7"/>
       <c r="W43" s="7"/>
     </row>
-    <row r="44" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" s="18"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
@@ -3048,7 +3423,7 @@
       <c r="V44" s="7"/>
       <c r="W44" s="7"/>
     </row>
-    <row r="45" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C45" s="18"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -3071,7 +3446,7 @@
       <c r="V45" s="7"/>
       <c r="W45" s="7"/>
     </row>
-    <row r="46" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C46" s="18"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
@@ -3094,7 +3469,7 @@
       <c r="V46" s="7"/>
       <c r="W46" s="7"/>
     </row>
-    <row r="47" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C47" s="18"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
@@ -3117,7 +3492,7 @@
       <c r="V47" s="7"/>
       <c r="W47" s="7"/>
     </row>
-    <row r="48" spans="3:23" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:25" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C48" s="18"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>

</xml_diff>

<commit_message>
chore: update param tracking file]
</commit_message>
<xml_diff>
--- a/Model_Param_Tracking.xlsx
+++ b/Model_Param_Tracking.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlotte/Desktop/Dissertation_Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2A775BC8-F713-D344-B9FB-088552282622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{41EA3D7E-79DE-D746-B70E-E95EE026C274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{93C3F197-1E59-6347-8491-F25656B50BA9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{93C3F197-1E59-6347-8491-F25656B50BA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Param_Tracking" sheetId="1" r:id="rId1"/>
+    <sheet name="All Stations Metrics Tracking" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="139">
   <si>
     <t>heads_gat</t>
   </si>
@@ -285,6 +286,174 @@
   </si>
   <si>
     <t>High Var</t>
+  </si>
+  <si>
+    <t>Station Name</t>
+  </si>
+  <si>
+    <t>Run ID</t>
+  </si>
+  <si>
+    <t>Run Timecode</t>
+  </si>
+  <si>
+    <t>run_GAT</t>
+  </si>
+  <si>
+    <t>run_LSTM</t>
+  </si>
+  <si>
+    <t>Node ID</t>
+  </si>
+  <si>
+    <t>ainstable</t>
+  </si>
+  <si>
+    <t>Val Station 1</t>
+  </si>
+  <si>
+    <t>Val Station 2</t>
+  </si>
+  <si>
+    <t>castle_carrock</t>
+  </si>
+  <si>
+    <t>skirwith</t>
+  </si>
+  <si>
+    <t>RMAE</t>
+  </si>
+  <si>
+    <t>R^2</t>
+  </si>
+  <si>
+    <t>NSE</t>
+  </si>
+  <si>
+    <t>KGE</t>
+  </si>
+  <si>
+    <t>GAT only</t>
+  </si>
+  <si>
+    <t>GAT + LSTM + Sigmoid Gate</t>
+  </si>
+  <si>
+    <t>feature/graph-conditioned-film</t>
+  </si>
+  <si>
+    <t>feature/gat-lstm-parallel-attention-new</t>
+  </si>
+  <si>
+    <t>Git Branch</t>
+  </si>
+  <si>
+    <t>LSTM only (No FiLM)</t>
+  </si>
+  <si>
+    <t>baronwood</t>
+  </si>
+  <si>
+    <t>bgs_ev2</t>
+  </si>
+  <si>
+    <t>cliburn_town_bridge_2</t>
+  </si>
+  <si>
+    <t>coupland</t>
+  </si>
+  <si>
+    <t>croglin</t>
+  </si>
+  <si>
+    <t>east_brownrigg</t>
+  </si>
+  <si>
+    <t>great_musgrave</t>
+  </si>
+  <si>
+    <t>hilton</t>
+  </si>
+  <si>
+    <t>longtown</t>
+  </si>
+  <si>
+    <t>penrith_north</t>
+  </si>
+  <si>
+    <t>renwick</t>
+  </si>
+  <si>
+    <t>scaleby</t>
+  </si>
+  <si>
+    <t>lstm_enabled</t>
+  </si>
+  <si>
+    <t>gat_enabled</t>
+  </si>
+  <si>
+    <t>film_mode</t>
+  </si>
+  <si>
+    <t>fusion_mode</t>
+  </si>
+  <si>
+    <t>film_graph_edges</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>NODE</t>
+  </si>
+  <si>
+    <t>GRAPH</t>
+  </si>
+  <si>
+    <t>GAT + LSTM + GAT Conditioned FiLM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temporal Only </t>
+  </si>
+  <si>
+    <t>LSTM_input</t>
+  </si>
+  <si>
+    <t>GAT_input</t>
+  </si>
+  <si>
+    <t>Static and Temporal</t>
+  </si>
+  <si>
+    <t>Static Only</t>
+  </si>
+  <si>
+    <t>GAT + LSTM + Node-wise FiLM + Sigmoid Gate</t>
+  </si>
+  <si>
+    <t>Performance Notes</t>
+  </si>
+  <si>
+    <t>GAT + LSTM with Node-wise FiLM + Sigmoid Gate</t>
+  </si>
+  <si>
+    <t>Baseline: MLP</t>
+  </si>
+  <si>
+    <t>Baseline: Fourier (Seasonal climatology)</t>
+  </si>
+  <si>
+    <t>SIGMOID GATE</t>
+  </si>
+  <si>
+    <t>GAT with Temporal Inputs (non Recurrent)</t>
+  </si>
+  <si>
+    <t>Ablations</t>
   </si>
 </sst>
 </file>
@@ -295,7 +464,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -350,8 +519,26 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -376,8 +563,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -400,11 +599,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -555,6 +769,66 @@
     </xf>
     <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BF201A-EBF7-3F4F-9E79-53BC4C3A4D14}">
   <dimension ref="B3:Z311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="83" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9545,4 +9819,1912 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1F69EA-4BBB-414D-9F90-38D180B1E811}">
+  <dimension ref="A2:AC72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="54"/>
+    <col min="2" max="2" width="19.5" style="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="59" customWidth="1"/>
+    <col min="4" max="5" width="19.5" style="54" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="54" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" style="54" customWidth="1"/>
+    <col min="8" max="8" width="2.5" style="54" customWidth="1"/>
+    <col min="9" max="9" width="40" style="54" customWidth="1"/>
+    <col min="10" max="10" width="34" style="54" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.5" style="54" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="55" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" style="55" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" style="55" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="15.6640625" style="55" customWidth="1"/>
+    <col min="18" max="18" width="18.1640625" style="55" customWidth="1"/>
+    <col min="19" max="19" width="2.5" style="54" hidden="1" customWidth="1"/>
+    <col min="20" max="21" width="0" style="64" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="2.5" style="54" customWidth="1"/>
+    <col min="23" max="27" width="13.33203125" style="54" customWidth="1"/>
+    <col min="28" max="28" width="2.33203125" style="54" customWidth="1"/>
+    <col min="29" max="29" width="52.33203125" style="64" customWidth="1"/>
+    <col min="30" max="16384" width="10.83203125" style="54"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:29" s="53" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="J2" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="M2" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="N2" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="O2" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="P2" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q2" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="R2" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="T2" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="U2" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="W2" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="X2" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y2" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z2" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA2" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC2" s="63" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:29" s="64" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="66">
+        <v>1335</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="I4" s="65" t="s">
+        <v>133</v>
+      </c>
+      <c r="J4" s="65" t="s">
+        <v>101</v>
+      </c>
+      <c r="L4" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="M4" s="67" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="O4" s="67" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q4" s="68" t="s">
+        <v>136</v>
+      </c>
+      <c r="R4" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="T4" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U4" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W4" s="65"/>
+      <c r="X4" s="65"/>
+      <c r="Y4" s="65"/>
+      <c r="Z4" s="65"/>
+      <c r="AA4" s="65"/>
+      <c r="AC4" s="65"/>
+    </row>
+    <row r="5" spans="1:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:29" s="70" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="54"/>
+      <c r="B6" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="60">
+        <v>1335</v>
+      </c>
+      <c r="D6" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="56"/>
+      <c r="G6" s="69"/>
+      <c r="I6" s="69" t="s">
+        <v>134</v>
+      </c>
+      <c r="J6" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="L6" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="M6" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="N6" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="O6" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="P6" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q6" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="R6" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="T6" s="69"/>
+      <c r="U6" s="69"/>
+      <c r="W6" s="69"/>
+      <c r="X6" s="69"/>
+      <c r="Y6" s="69"/>
+      <c r="Z6" s="69"/>
+      <c r="AA6" s="69"/>
+      <c r="AC6" s="69"/>
+    </row>
+    <row r="7" spans="1:29" s="64" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="66">
+        <v>1335</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="I7" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="J7" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="L7" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="M7" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="N7" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="O7" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="P7" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q7" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="R7" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="T7" s="65"/>
+      <c r="U7" s="65"/>
+      <c r="W7" s="65"/>
+      <c r="X7" s="65"/>
+      <c r="Y7" s="65"/>
+      <c r="Z7" s="65"/>
+      <c r="AA7" s="65"/>
+      <c r="AC7" s="65"/>
+    </row>
+    <row r="8" spans="1:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="60">
+        <v>1335</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="I9" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="J9" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="M9" s="57" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="O9" s="57" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q9" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="R9" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="T9" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U9" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W9" s="56"/>
+      <c r="X9" s="56"/>
+      <c r="Y9" s="56"/>
+      <c r="Z9" s="56"/>
+      <c r="AA9" s="56"/>
+      <c r="AC9" s="65"/>
+    </row>
+    <row r="10" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="60">
+        <v>1335</v>
+      </c>
+      <c r="D10" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="I10" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="J10" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="M10" s="57" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="O10" s="57" t="b">
+        <v>0</v>
+      </c>
+      <c r="P10" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q10" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="R10" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="T10" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U10" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W10" s="56"/>
+      <c r="X10" s="56"/>
+      <c r="Y10" s="56"/>
+      <c r="Z10" s="56"/>
+      <c r="AA10" s="56"/>
+      <c r="AC10" s="65"/>
+    </row>
+    <row r="11" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="51"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="I11" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="J11" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="57"/>
+      <c r="T11" s="65"/>
+      <c r="U11" s="65"/>
+      <c r="W11" s="56"/>
+      <c r="X11" s="56"/>
+      <c r="Y11" s="56"/>
+      <c r="Z11" s="56"/>
+      <c r="AA11" s="56"/>
+      <c r="AC11" s="65"/>
+    </row>
+    <row r="12" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="60">
+        <v>1335</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="I12" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="J12" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="L12" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="M12" s="57" t="b">
+        <v>1</v>
+      </c>
+      <c r="N12" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="O12" s="57" t="b">
+        <v>1</v>
+      </c>
+      <c r="P12" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q12" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="R12" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="T12" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U12" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W12" s="56"/>
+      <c r="X12" s="56"/>
+      <c r="Y12" s="56"/>
+      <c r="Z12" s="56"/>
+      <c r="AA12" s="56"/>
+      <c r="AC12" s="65"/>
+    </row>
+    <row r="13" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="60">
+        <v>1335</v>
+      </c>
+      <c r="D13" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="I13" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="J13" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="M13" s="57" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="O13" s="57" t="b">
+        <v>1</v>
+      </c>
+      <c r="P13" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q13" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="R13" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="T13" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U13" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W13" s="56"/>
+      <c r="X13" s="56"/>
+      <c r="Y13" s="56"/>
+      <c r="Z13" s="56"/>
+      <c r="AA13" s="56"/>
+      <c r="AC13" s="65"/>
+    </row>
+    <row r="14" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="60">
+        <v>1335</v>
+      </c>
+      <c r="D14" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="I14" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="J14" s="62" t="s">
+        <v>100</v>
+      </c>
+      <c r="L14" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="M14" s="57" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="O14" s="57" t="b">
+        <v>1</v>
+      </c>
+      <c r="P14" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q14" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="R14" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="T14" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U14" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W14" s="56"/>
+      <c r="X14" s="56"/>
+      <c r="Y14" s="56"/>
+      <c r="Z14" s="56"/>
+      <c r="AA14" s="56"/>
+      <c r="AC14" s="65"/>
+    </row>
+    <row r="15" spans="1:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="60"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="57"/>
+      <c r="R16" s="57"/>
+      <c r="T16" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U16" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W16" s="56"/>
+      <c r="X16" s="56"/>
+      <c r="Y16" s="56"/>
+      <c r="Z16" s="56"/>
+      <c r="AA16" s="56"/>
+      <c r="AC16" s="65"/>
+    </row>
+    <row r="17" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="60"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="57"/>
+      <c r="N17" s="57"/>
+      <c r="O17" s="57"/>
+      <c r="P17" s="57"/>
+      <c r="Q17" s="57"/>
+      <c r="R17" s="57"/>
+      <c r="T17" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U17" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W17" s="56"/>
+      <c r="X17" s="56"/>
+      <c r="Y17" s="56"/>
+      <c r="Z17" s="56"/>
+      <c r="AA17" s="56"/>
+      <c r="AC17" s="65"/>
+    </row>
+    <row r="18" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="60"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="57"/>
+      <c r="Q18" s="57"/>
+      <c r="R18" s="57"/>
+      <c r="T18" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U18" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W18" s="56"/>
+      <c r="X18" s="56"/>
+      <c r="Y18" s="56"/>
+      <c r="Z18" s="56"/>
+      <c r="AA18" s="56"/>
+      <c r="AC18" s="65"/>
+    </row>
+    <row r="19" spans="2:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="60"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="56"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="57"/>
+      <c r="N20" s="57"/>
+      <c r="O20" s="57"/>
+      <c r="P20" s="57"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="57"/>
+      <c r="T20" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U20" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W20" s="56"/>
+      <c r="X20" s="56"/>
+      <c r="Y20" s="56"/>
+      <c r="Z20" s="56"/>
+      <c r="AA20" s="56"/>
+      <c r="AC20" s="65"/>
+    </row>
+    <row r="21" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="60"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="57"/>
+      <c r="P21" s="57"/>
+      <c r="Q21" s="57"/>
+      <c r="R21" s="57"/>
+      <c r="T21" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U21" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W21" s="56"/>
+      <c r="X21" s="56"/>
+      <c r="Y21" s="56"/>
+      <c r="Z21" s="56"/>
+      <c r="AA21" s="56"/>
+      <c r="AC21" s="65"/>
+    </row>
+    <row r="22" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="60"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="57"/>
+      <c r="P22" s="57"/>
+      <c r="Q22" s="57"/>
+      <c r="R22" s="57"/>
+      <c r="T22" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U22" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W22" s="56"/>
+      <c r="X22" s="56"/>
+      <c r="Y22" s="56"/>
+      <c r="Z22" s="56"/>
+      <c r="AA22" s="56"/>
+      <c r="AC22" s="65"/>
+    </row>
+    <row r="23" spans="2:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="60"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="56"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="57"/>
+      <c r="O24" s="57"/>
+      <c r="P24" s="57"/>
+      <c r="Q24" s="57"/>
+      <c r="R24" s="57"/>
+      <c r="T24" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U24" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W24" s="56"/>
+      <c r="X24" s="56"/>
+      <c r="Y24" s="56"/>
+      <c r="Z24" s="56"/>
+      <c r="AA24" s="56"/>
+      <c r="AC24" s="65"/>
+    </row>
+    <row r="25" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="60"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="56"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="57"/>
+      <c r="P25" s="57"/>
+      <c r="Q25" s="57"/>
+      <c r="R25" s="57"/>
+      <c r="T25" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U25" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W25" s="56"/>
+      <c r="X25" s="56"/>
+      <c r="Y25" s="56"/>
+      <c r="Z25" s="56"/>
+      <c r="AA25" s="56"/>
+      <c r="AC25" s="65"/>
+    </row>
+    <row r="26" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="60"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="57"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="57"/>
+      <c r="P26" s="57"/>
+      <c r="Q26" s="57"/>
+      <c r="R26" s="57"/>
+      <c r="T26" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U26" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W26" s="56"/>
+      <c r="X26" s="56"/>
+      <c r="Y26" s="56"/>
+      <c r="Z26" s="56"/>
+      <c r="AA26" s="56"/>
+      <c r="AC26" s="65"/>
+    </row>
+    <row r="27" spans="2:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="60"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="L28" s="57"/>
+      <c r="M28" s="57"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="57"/>
+      <c r="P28" s="57"/>
+      <c r="Q28" s="57"/>
+      <c r="R28" s="57"/>
+      <c r="T28" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U28" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W28" s="56"/>
+      <c r="X28" s="56"/>
+      <c r="Y28" s="56"/>
+      <c r="Z28" s="56"/>
+      <c r="AA28" s="56"/>
+      <c r="AC28" s="65"/>
+    </row>
+    <row r="29" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="60"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="56"/>
+      <c r="L29" s="57"/>
+      <c r="M29" s="57"/>
+      <c r="N29" s="57"/>
+      <c r="O29" s="57"/>
+      <c r="P29" s="57"/>
+      <c r="Q29" s="57"/>
+      <c r="R29" s="57"/>
+      <c r="T29" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U29" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W29" s="56"/>
+      <c r="X29" s="56"/>
+      <c r="Y29" s="56"/>
+      <c r="Z29" s="56"/>
+      <c r="AA29" s="56"/>
+      <c r="AC29" s="65"/>
+    </row>
+    <row r="30" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="60"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
+      <c r="L30" s="57"/>
+      <c r="M30" s="57"/>
+      <c r="N30" s="57"/>
+      <c r="O30" s="57"/>
+      <c r="P30" s="57"/>
+      <c r="Q30" s="57"/>
+      <c r="R30" s="57"/>
+      <c r="T30" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U30" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W30" s="56"/>
+      <c r="X30" s="56"/>
+      <c r="Y30" s="56"/>
+      <c r="Z30" s="56"/>
+      <c r="AA30" s="56"/>
+      <c r="AC30" s="65"/>
+    </row>
+    <row r="31" spans="2:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" s="60"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="L32" s="57"/>
+      <c r="M32" s="57"/>
+      <c r="N32" s="57"/>
+      <c r="O32" s="57"/>
+      <c r="P32" s="57"/>
+      <c r="Q32" s="57"/>
+      <c r="R32" s="57"/>
+      <c r="T32" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U32" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W32" s="56"/>
+      <c r="X32" s="56"/>
+      <c r="Y32" s="56"/>
+      <c r="Z32" s="56"/>
+      <c r="AA32" s="56"/>
+      <c r="AC32" s="65"/>
+    </row>
+    <row r="33" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="60"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
+      <c r="L33" s="57"/>
+      <c r="M33" s="57"/>
+      <c r="N33" s="57"/>
+      <c r="O33" s="57"/>
+      <c r="P33" s="57"/>
+      <c r="Q33" s="57"/>
+      <c r="R33" s="57"/>
+      <c r="T33" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U33" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W33" s="56"/>
+      <c r="X33" s="56"/>
+      <c r="Y33" s="56"/>
+      <c r="Z33" s="56"/>
+      <c r="AA33" s="56"/>
+      <c r="AC33" s="65"/>
+    </row>
+    <row r="34" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="60"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
+      <c r="I34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="L34" s="57"/>
+      <c r="M34" s="57"/>
+      <c r="N34" s="57"/>
+      <c r="O34" s="57"/>
+      <c r="P34" s="57"/>
+      <c r="Q34" s="57"/>
+      <c r="R34" s="57"/>
+      <c r="T34" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U34" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W34" s="56"/>
+      <c r="X34" s="56"/>
+      <c r="Y34" s="56"/>
+      <c r="Z34" s="56"/>
+      <c r="AA34" s="56"/>
+      <c r="AC34" s="65"/>
+    </row>
+    <row r="35" spans="2:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="60"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="I36" s="56"/>
+      <c r="J36" s="56"/>
+      <c r="L36" s="57"/>
+      <c r="M36" s="57"/>
+      <c r="N36" s="57"/>
+      <c r="O36" s="57"/>
+      <c r="P36" s="57"/>
+      <c r="Q36" s="57"/>
+      <c r="R36" s="57"/>
+      <c r="T36" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U36" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W36" s="56"/>
+      <c r="X36" s="56"/>
+      <c r="Y36" s="56"/>
+      <c r="Z36" s="56"/>
+      <c r="AA36" s="56"/>
+      <c r="AC36" s="65"/>
+    </row>
+    <row r="37" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="60"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="56"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="56"/>
+      <c r="L37" s="57"/>
+      <c r="M37" s="57"/>
+      <c r="N37" s="57"/>
+      <c r="O37" s="57"/>
+      <c r="P37" s="57"/>
+      <c r="Q37" s="57"/>
+      <c r="R37" s="57"/>
+      <c r="T37" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U37" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W37" s="56"/>
+      <c r="X37" s="56"/>
+      <c r="Y37" s="56"/>
+      <c r="Z37" s="56"/>
+      <c r="AA37" s="56"/>
+      <c r="AC37" s="65"/>
+    </row>
+    <row r="38" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="60"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="56"/>
+      <c r="I38" s="56"/>
+      <c r="J38" s="56"/>
+      <c r="L38" s="57"/>
+      <c r="M38" s="57"/>
+      <c r="N38" s="57"/>
+      <c r="O38" s="57"/>
+      <c r="P38" s="57"/>
+      <c r="Q38" s="57"/>
+      <c r="R38" s="57"/>
+      <c r="T38" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U38" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W38" s="56"/>
+      <c r="X38" s="56"/>
+      <c r="Y38" s="56"/>
+      <c r="Z38" s="56"/>
+      <c r="AA38" s="56"/>
+      <c r="AC38" s="65"/>
+    </row>
+    <row r="39" spans="2:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="60"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="56"/>
+      <c r="I40" s="56"/>
+      <c r="J40" s="56"/>
+      <c r="L40" s="57"/>
+      <c r="M40" s="57"/>
+      <c r="N40" s="57"/>
+      <c r="O40" s="57"/>
+      <c r="P40" s="57"/>
+      <c r="Q40" s="57"/>
+      <c r="R40" s="57"/>
+      <c r="T40" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U40" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W40" s="56"/>
+      <c r="X40" s="56"/>
+      <c r="Y40" s="56"/>
+      <c r="Z40" s="56"/>
+      <c r="AA40" s="56"/>
+      <c r="AC40" s="65"/>
+    </row>
+    <row r="41" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="60"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="56"/>
+      <c r="G41" s="56"/>
+      <c r="I41" s="56"/>
+      <c r="J41" s="56"/>
+      <c r="L41" s="57"/>
+      <c r="M41" s="57"/>
+      <c r="N41" s="57"/>
+      <c r="O41" s="57"/>
+      <c r="P41" s="57"/>
+      <c r="Q41" s="57"/>
+      <c r="R41" s="57"/>
+      <c r="T41" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U41" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W41" s="56"/>
+      <c r="X41" s="56"/>
+      <c r="Y41" s="56"/>
+      <c r="Z41" s="56"/>
+      <c r="AA41" s="56"/>
+      <c r="AC41" s="65"/>
+    </row>
+    <row r="42" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="60"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="56"/>
+      <c r="I42" s="56"/>
+      <c r="J42" s="56"/>
+      <c r="L42" s="57"/>
+      <c r="M42" s="57"/>
+      <c r="N42" s="57"/>
+      <c r="O42" s="57"/>
+      <c r="P42" s="57"/>
+      <c r="Q42" s="57"/>
+      <c r="R42" s="57"/>
+      <c r="T42" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U42" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W42" s="56"/>
+      <c r="X42" s="56"/>
+      <c r="Y42" s="56"/>
+      <c r="Z42" s="56"/>
+      <c r="AA42" s="56"/>
+      <c r="AC42" s="65"/>
+    </row>
+    <row r="43" spans="2:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" s="60"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="56"/>
+      <c r="F44" s="56"/>
+      <c r="G44" s="56"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="56"/>
+      <c r="L44" s="57"/>
+      <c r="M44" s="57"/>
+      <c r="N44" s="57"/>
+      <c r="O44" s="57"/>
+      <c r="P44" s="57"/>
+      <c r="Q44" s="57"/>
+      <c r="R44" s="57"/>
+      <c r="T44" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U44" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W44" s="56"/>
+      <c r="X44" s="56"/>
+      <c r="Y44" s="56"/>
+      <c r="Z44" s="56"/>
+      <c r="AA44" s="56"/>
+      <c r="AC44" s="65"/>
+    </row>
+    <row r="45" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="60"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="L45" s="57"/>
+      <c r="M45" s="57"/>
+      <c r="N45" s="57"/>
+      <c r="O45" s="57"/>
+      <c r="P45" s="57"/>
+      <c r="Q45" s="57"/>
+      <c r="R45" s="57"/>
+      <c r="T45" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U45" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W45" s="56"/>
+      <c r="X45" s="56"/>
+      <c r="Y45" s="56"/>
+      <c r="Z45" s="56"/>
+      <c r="AA45" s="56"/>
+      <c r="AC45" s="65"/>
+    </row>
+    <row r="46" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" s="60"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="56"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
+      <c r="L46" s="57"/>
+      <c r="M46" s="57"/>
+      <c r="N46" s="57"/>
+      <c r="O46" s="57"/>
+      <c r="P46" s="57"/>
+      <c r="Q46" s="57"/>
+      <c r="R46" s="57"/>
+      <c r="T46" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U46" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W46" s="56"/>
+      <c r="X46" s="56"/>
+      <c r="Y46" s="56"/>
+      <c r="Z46" s="56"/>
+      <c r="AA46" s="56"/>
+      <c r="AC46" s="65"/>
+    </row>
+    <row r="47" spans="2:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="60"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="56"/>
+      <c r="I48" s="56"/>
+      <c r="J48" s="56"/>
+      <c r="L48" s="57"/>
+      <c r="M48" s="57"/>
+      <c r="N48" s="57"/>
+      <c r="O48" s="57"/>
+      <c r="P48" s="57"/>
+      <c r="Q48" s="57"/>
+      <c r="R48" s="57"/>
+      <c r="T48" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U48" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W48" s="56"/>
+      <c r="X48" s="56"/>
+      <c r="Y48" s="56"/>
+      <c r="Z48" s="56"/>
+      <c r="AA48" s="56"/>
+      <c r="AC48" s="65"/>
+    </row>
+    <row r="49" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" s="60"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="56"/>
+      <c r="G49" s="56"/>
+      <c r="I49" s="56"/>
+      <c r="J49" s="56"/>
+      <c r="L49" s="57"/>
+      <c r="M49" s="57"/>
+      <c r="N49" s="57"/>
+      <c r="O49" s="57"/>
+      <c r="P49" s="57"/>
+      <c r="Q49" s="57"/>
+      <c r="R49" s="57"/>
+      <c r="T49" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U49" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W49" s="56"/>
+      <c r="X49" s="56"/>
+      <c r="Y49" s="56"/>
+      <c r="Z49" s="56"/>
+      <c r="AA49" s="56"/>
+      <c r="AC49" s="65"/>
+    </row>
+    <row r="50" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" s="60"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="56"/>
+      <c r="G50" s="56"/>
+      <c r="I50" s="56"/>
+      <c r="J50" s="56"/>
+      <c r="L50" s="57"/>
+      <c r="M50" s="57"/>
+      <c r="N50" s="57"/>
+      <c r="O50" s="57"/>
+      <c r="P50" s="57"/>
+      <c r="Q50" s="57"/>
+      <c r="R50" s="57"/>
+      <c r="T50" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U50" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W50" s="56"/>
+      <c r="X50" s="56"/>
+      <c r="Y50" s="56"/>
+      <c r="Z50" s="56"/>
+      <c r="AA50" s="56"/>
+      <c r="AC50" s="65"/>
+    </row>
+    <row r="51" spans="2:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" s="60"/>
+      <c r="D52" s="56"/>
+      <c r="E52" s="56"/>
+      <c r="F52" s="56"/>
+      <c r="G52" s="56"/>
+      <c r="I52" s="56"/>
+      <c r="J52" s="56"/>
+      <c r="L52" s="57"/>
+      <c r="M52" s="57"/>
+      <c r="N52" s="57"/>
+      <c r="O52" s="57"/>
+      <c r="P52" s="57"/>
+      <c r="Q52" s="57"/>
+      <c r="R52" s="57"/>
+      <c r="T52" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U52" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W52" s="56"/>
+      <c r="X52" s="56"/>
+      <c r="Y52" s="56"/>
+      <c r="Z52" s="56"/>
+      <c r="AA52" s="56"/>
+      <c r="AC52" s="65"/>
+    </row>
+    <row r="53" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="60"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="56"/>
+      <c r="I53" s="56"/>
+      <c r="J53" s="56"/>
+      <c r="L53" s="57"/>
+      <c r="M53" s="57"/>
+      <c r="N53" s="57"/>
+      <c r="O53" s="57"/>
+      <c r="P53" s="57"/>
+      <c r="Q53" s="57"/>
+      <c r="R53" s="57"/>
+      <c r="T53" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U53" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W53" s="56"/>
+      <c r="X53" s="56"/>
+      <c r="Y53" s="56"/>
+      <c r="Z53" s="56"/>
+      <c r="AA53" s="56"/>
+      <c r="AC53" s="65"/>
+    </row>
+    <row r="54" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="60"/>
+      <c r="D54" s="56"/>
+      <c r="E54" s="56"/>
+      <c r="F54" s="56"/>
+      <c r="G54" s="56"/>
+      <c r="I54" s="56"/>
+      <c r="J54" s="56"/>
+      <c r="L54" s="57"/>
+      <c r="M54" s="57"/>
+      <c r="N54" s="57"/>
+      <c r="O54" s="57"/>
+      <c r="P54" s="57"/>
+      <c r="Q54" s="57"/>
+      <c r="R54" s="57"/>
+      <c r="T54" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U54" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W54" s="56"/>
+      <c r="X54" s="56"/>
+      <c r="Y54" s="56"/>
+      <c r="Z54" s="56"/>
+      <c r="AA54" s="56"/>
+      <c r="AC54" s="65"/>
+    </row>
+    <row r="55" spans="2:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" s="60"/>
+      <c r="D56" s="56"/>
+      <c r="E56" s="56"/>
+      <c r="F56" s="56"/>
+      <c r="G56" s="56"/>
+      <c r="I56" s="56"/>
+      <c r="J56" s="56"/>
+      <c r="L56" s="57"/>
+      <c r="M56" s="57"/>
+      <c r="N56" s="57"/>
+      <c r="O56" s="57"/>
+      <c r="P56" s="57"/>
+      <c r="Q56" s="57"/>
+      <c r="R56" s="57"/>
+      <c r="T56" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U56" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W56" s="56"/>
+      <c r="X56" s="56"/>
+      <c r="Y56" s="56"/>
+      <c r="Z56" s="56"/>
+      <c r="AA56" s="56"/>
+      <c r="AC56" s="65"/>
+    </row>
+    <row r="57" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" s="60"/>
+      <c r="D57" s="56"/>
+      <c r="E57" s="56"/>
+      <c r="F57" s="56"/>
+      <c r="G57" s="56"/>
+      <c r="I57" s="56"/>
+      <c r="J57" s="56"/>
+      <c r="L57" s="57"/>
+      <c r="M57" s="57"/>
+      <c r="N57" s="57"/>
+      <c r="O57" s="57"/>
+      <c r="P57" s="57"/>
+      <c r="Q57" s="57"/>
+      <c r="R57" s="57"/>
+      <c r="T57" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U57" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W57" s="56"/>
+      <c r="X57" s="56"/>
+      <c r="Y57" s="56"/>
+      <c r="Z57" s="56"/>
+      <c r="AA57" s="56"/>
+      <c r="AC57" s="65"/>
+    </row>
+    <row r="58" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="60"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="56"/>
+      <c r="F58" s="56"/>
+      <c r="G58" s="56"/>
+      <c r="I58" s="56"/>
+      <c r="J58" s="56"/>
+      <c r="L58" s="57"/>
+      <c r="M58" s="57"/>
+      <c r="N58" s="57"/>
+      <c r="O58" s="57"/>
+      <c r="P58" s="57"/>
+      <c r="Q58" s="57"/>
+      <c r="R58" s="57"/>
+      <c r="T58" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U58" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W58" s="56"/>
+      <c r="X58" s="56"/>
+      <c r="Y58" s="56"/>
+      <c r="Z58" s="56"/>
+      <c r="AA58" s="56"/>
+      <c r="AC58" s="65"/>
+    </row>
+    <row r="59" spans="2:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" s="60"/>
+      <c r="D60" s="56"/>
+      <c r="E60" s="56"/>
+      <c r="F60" s="56"/>
+      <c r="G60" s="56"/>
+      <c r="I60" s="56"/>
+      <c r="J60" s="56"/>
+      <c r="L60" s="57"/>
+      <c r="M60" s="57"/>
+      <c r="N60" s="57"/>
+      <c r="O60" s="57"/>
+      <c r="P60" s="57"/>
+      <c r="Q60" s="57"/>
+      <c r="R60" s="57"/>
+      <c r="T60" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U60" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W60" s="56"/>
+      <c r="X60" s="56"/>
+      <c r="Y60" s="56"/>
+      <c r="Z60" s="56"/>
+      <c r="AA60" s="56"/>
+      <c r="AC60" s="65"/>
+    </row>
+    <row r="61" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C61" s="60"/>
+      <c r="D61" s="56"/>
+      <c r="E61" s="56"/>
+      <c r="F61" s="56"/>
+      <c r="G61" s="56"/>
+      <c r="I61" s="56"/>
+      <c r="J61" s="56"/>
+      <c r="L61" s="57"/>
+      <c r="M61" s="57"/>
+      <c r="N61" s="57"/>
+      <c r="O61" s="57"/>
+      <c r="P61" s="57"/>
+      <c r="Q61" s="57"/>
+      <c r="R61" s="57"/>
+      <c r="T61" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U61" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W61" s="56"/>
+      <c r="X61" s="56"/>
+      <c r="Y61" s="56"/>
+      <c r="Z61" s="56"/>
+      <c r="AA61" s="56"/>
+      <c r="AC61" s="65"/>
+    </row>
+    <row r="62" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62" s="60"/>
+      <c r="D62" s="56"/>
+      <c r="E62" s="56"/>
+      <c r="F62" s="56"/>
+      <c r="G62" s="56"/>
+      <c r="I62" s="56"/>
+      <c r="J62" s="56"/>
+      <c r="L62" s="57"/>
+      <c r="M62" s="57"/>
+      <c r="N62" s="57"/>
+      <c r="O62" s="57"/>
+      <c r="P62" s="57"/>
+      <c r="Q62" s="57"/>
+      <c r="R62" s="57"/>
+      <c r="T62" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U62" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W62" s="56"/>
+      <c r="X62" s="56"/>
+      <c r="Y62" s="56"/>
+      <c r="Z62" s="56"/>
+      <c r="AA62" s="56"/>
+      <c r="AC62" s="65"/>
+    </row>
+    <row r="63" spans="2:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="C64" s="60"/>
+      <c r="D64" s="56"/>
+      <c r="E64" s="56"/>
+      <c r="F64" s="56"/>
+      <c r="G64" s="56"/>
+      <c r="I64" s="56"/>
+      <c r="J64" s="56"/>
+      <c r="L64" s="57"/>
+      <c r="M64" s="57"/>
+      <c r="N64" s="57"/>
+      <c r="O64" s="57"/>
+      <c r="P64" s="57"/>
+      <c r="Q64" s="57"/>
+      <c r="R64" s="57"/>
+      <c r="T64" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U64" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W64" s="56"/>
+      <c r="X64" s="56"/>
+      <c r="Y64" s="56"/>
+      <c r="Z64" s="56"/>
+      <c r="AA64" s="56"/>
+      <c r="AC64" s="65"/>
+    </row>
+    <row r="65" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="C65" s="60"/>
+      <c r="D65" s="56"/>
+      <c r="E65" s="56"/>
+      <c r="F65" s="56"/>
+      <c r="G65" s="56"/>
+      <c r="I65" s="56"/>
+      <c r="J65" s="56"/>
+      <c r="L65" s="57"/>
+      <c r="M65" s="57"/>
+      <c r="N65" s="57"/>
+      <c r="O65" s="57"/>
+      <c r="P65" s="57"/>
+      <c r="Q65" s="57"/>
+      <c r="R65" s="57"/>
+      <c r="T65" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U65" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W65" s="56"/>
+      <c r="X65" s="56"/>
+      <c r="Y65" s="56"/>
+      <c r="Z65" s="56"/>
+      <c r="AA65" s="56"/>
+      <c r="AC65" s="65"/>
+    </row>
+    <row r="66" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66" s="60"/>
+      <c r="D66" s="56"/>
+      <c r="E66" s="56"/>
+      <c r="F66" s="56"/>
+      <c r="G66" s="56"/>
+      <c r="I66" s="56"/>
+      <c r="J66" s="56"/>
+      <c r="L66" s="57"/>
+      <c r="M66" s="57"/>
+      <c r="N66" s="57"/>
+      <c r="O66" s="57"/>
+      <c r="P66" s="57"/>
+      <c r="Q66" s="57"/>
+      <c r="R66" s="57"/>
+      <c r="T66" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U66" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W66" s="56"/>
+      <c r="X66" s="56"/>
+      <c r="Y66" s="56"/>
+      <c r="Z66" s="56"/>
+      <c r="AA66" s="56"/>
+      <c r="AC66" s="65"/>
+    </row>
+    <row r="67" spans="2:29" ht="11" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C68" s="60"/>
+      <c r="D68" s="56"/>
+      <c r="E68" s="56"/>
+      <c r="F68" s="56"/>
+      <c r="G68" s="56"/>
+      <c r="I68" s="56"/>
+      <c r="J68" s="56"/>
+      <c r="L68" s="57"/>
+      <c r="M68" s="57"/>
+      <c r="N68" s="57"/>
+      <c r="O68" s="57"/>
+      <c r="P68" s="57"/>
+      <c r="Q68" s="57"/>
+      <c r="R68" s="57"/>
+      <c r="T68" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U68" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="W68" s="56"/>
+      <c r="X68" s="56"/>
+      <c r="Y68" s="56"/>
+      <c r="Z68" s="56"/>
+      <c r="AA68" s="56"/>
+      <c r="AC68" s="65"/>
+    </row>
+    <row r="69" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C69" s="60"/>
+      <c r="D69" s="56"/>
+      <c r="E69" s="56"/>
+      <c r="F69" s="56"/>
+      <c r="G69" s="56"/>
+      <c r="I69" s="56"/>
+      <c r="J69" s="56"/>
+      <c r="L69" s="57"/>
+      <c r="M69" s="57"/>
+      <c r="N69" s="57"/>
+      <c r="O69" s="57"/>
+      <c r="P69" s="57"/>
+      <c r="Q69" s="57"/>
+      <c r="R69" s="57"/>
+      <c r="T69" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="U69" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W69" s="56"/>
+      <c r="X69" s="56"/>
+      <c r="Y69" s="56"/>
+      <c r="Z69" s="56"/>
+      <c r="AA69" s="56"/>
+      <c r="AC69" s="65"/>
+    </row>
+    <row r="70" spans="2:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C70" s="60"/>
+      <c r="D70" s="56"/>
+      <c r="E70" s="56"/>
+      <c r="F70" s="56"/>
+      <c r="G70" s="56"/>
+      <c r="I70" s="56"/>
+      <c r="J70" s="56"/>
+      <c r="L70" s="57"/>
+      <c r="M70" s="57"/>
+      <c r="N70" s="57"/>
+      <c r="O70" s="57"/>
+      <c r="P70" s="57"/>
+      <c r="Q70" s="57"/>
+      <c r="R70" s="57"/>
+      <c r="T70" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="U70" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="W70" s="56"/>
+      <c r="X70" s="56"/>
+      <c r="Y70" s="56"/>
+      <c r="Z70" s="56"/>
+      <c r="AA70" s="56"/>
+      <c r="AC70" s="65"/>
+    </row>
+    <row r="71" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="G71" s="61"/>
+      <c r="H71" s="61"/>
+      <c r="I71" s="61"/>
+      <c r="J71" s="61"/>
+      <c r="K71" s="61"/>
+      <c r="S71" s="61"/>
+    </row>
+    <row r="72" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="G72" s="61"/>
+      <c r="H72" s="61"/>
+      <c r="I72" s="61"/>
+      <c r="J72" s="61"/>
+      <c r="K72" s="61"/>
+      <c r="S72" s="61"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>